<commit_message>
Update RTM with the New SRS
</commit_message>
<xml_diff>
--- a/RTM/RTM.xlsx
+++ b/RTM/RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>SRS_00_5</t>
   </si>
@@ -32,12 +32,6 @@
     <t>SRS_00_6</t>
   </si>
   <si>
-    <t>CRS_00_6, CRS_00_10, CRS_00_11, CRS_00_12, CRS_00_13, CRS_00_14</t>
-  </si>
-  <si>
-    <t>CRS_00_2, CRS_00_5, CRS_00_7, CRS_00_8, CRS_00_9, CRS_00_11</t>
-  </si>
-  <si>
     <t>SRS_00_4</t>
   </si>
   <si>
@@ -56,9 +50,6 @@
     <t>SRS_00_1</t>
   </si>
   <si>
-    <t>CRS_00_4</t>
-  </si>
-  <si>
     <t>RELATED SRS</t>
   </si>
   <si>
@@ -78,6 +69,30 @@
   </si>
   <si>
     <t>RTM FOR FAN CONTROLLER SYSTEM</t>
+  </si>
+  <si>
+    <t>CRS_00_6</t>
+  </si>
+  <si>
+    <t>CRS_00_2, CRS_00_5</t>
+  </si>
+  <si>
+    <t>SRS_00_7</t>
+  </si>
+  <si>
+    <t>CRS_00_7, CRS_00_8, CRS_00_9, CRS_00_11</t>
+  </si>
+  <si>
+    <t>CRS_00_10</t>
+  </si>
+  <si>
+    <t>CRS_00_12, CRS_00_13, CRS_00_14</t>
+  </si>
+  <si>
+    <t>SRS_00_2, SRS_00_3</t>
+  </si>
+  <si>
+    <t>SRS_00_2, SRS_00_3, SRS_00_4</t>
   </si>
 </sst>
 </file>
@@ -122,7 +137,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -145,15 +160,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -165,6 +188,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -634,7 +660,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,123 +670,128 @@
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2" t="s">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2" t="s">
-        <v>0</v>
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update RTM with CDDs files
</commit_message>
<xml_diff>
--- a/RTM/RTM.xlsx
+++ b/RTM/RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>SRS_00_5</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>SRS_00_2, SRS_00_3, SRS_00_4</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>ADC-CDD.doc, ADC-CDD</t>
+  </si>
+  <si>
+    <t>LCD-CDD.doc, DIO-CDD.doc</t>
+  </si>
+  <si>
+    <t>App-CDD.doc</t>
   </si>
 </sst>
 </file>
@@ -175,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -187,11 +199,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -199,7 +224,8 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -212,12 +238,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -385,10 +405,10 @@
   <tableColumns count="6">
     <tableColumn id="1" name="CRS" dataDxfId="5"/>
     <tableColumn id="2" name="SRS" dataDxfId="4"/>
-    <tableColumn id="3" name="DESIGN" dataDxfId="3"/>
-    <tableColumn id="4" name="CODE" dataDxfId="2"/>
-    <tableColumn id="5" name="TEST" dataDxfId="1"/>
-    <tableColumn id="6" name="RELATED SRS" dataDxfId="0"/>
+    <tableColumn id="3" name="DESIGN" dataDxfId="0"/>
+    <tableColumn id="4" name="CODE" dataDxfId="3"/>
+    <tableColumn id="5" name="TEST" dataDxfId="2"/>
+    <tableColumn id="6" name="RELATED SRS" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -660,37 +680,36 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="83.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -704,37 +723,43 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="1" t="s">
@@ -748,7 +773,9 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="1" t="s">
@@ -762,7 +789,9 @@
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="1" t="s">
@@ -776,7 +805,9 @@
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="1"/>
@@ -788,10 +819,12 @@
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update the RTM with Code files
</commit_message>
<xml_diff>
--- a/RTM/RTM.xlsx
+++ b/RTM/RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>SRS_00_5</t>
   </si>
@@ -98,13 +98,31 @@
     <t>NA</t>
   </si>
   <si>
-    <t>ADC-CDD.doc, ADC-CDD</t>
-  </si>
-  <si>
     <t>LCD-CDD.doc, DIO-CDD.doc</t>
   </si>
   <si>
     <t>App-CDD.doc</t>
+  </si>
+  <si>
+    <t>ADC-CDD.doc, LM35-CDD</t>
+  </si>
+  <si>
+    <t>ADC_prog.c &amp; Volt_prog.c</t>
+  </si>
+  <si>
+    <t>LCD_prog.c &amp; DIO_prog.c</t>
+  </si>
+  <si>
+    <t>Application.c</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>App-CDD.doc &amp; LCD-CDD.doc &amp; DIO-CDD.doc</t>
+  </si>
+  <si>
+    <t>Application.c &amp; LCD_prog.c &amp; DIO_prog.c</t>
   </si>
 </sst>
 </file>
@@ -192,7 +210,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -200,31 +217,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -241,7 +264,8 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -254,16 +278,11 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -276,16 +295,11 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -298,12 +312,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -323,7 +331,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -336,12 +344,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -355,7 +357,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -368,8 +370,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -400,12 +400,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F8" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0">
   <autoFilter ref="A2:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="CRS" dataDxfId="5"/>
-    <tableColumn id="2" name="SRS" dataDxfId="4"/>
-    <tableColumn id="3" name="DESIGN" dataDxfId="0"/>
+    <tableColumn id="1" name="CRS" dataDxfId="6"/>
+    <tableColumn id="2" name="SRS" dataDxfId="5"/>
+    <tableColumn id="3" name="DESIGN" dataDxfId="4"/>
     <tableColumn id="4" name="CODE" dataDxfId="3"/>
     <tableColumn id="5" name="TEST" dataDxfId="2"/>
     <tableColumn id="6" name="RELATED SRS" dataDxfId="1"/>
@@ -677,91 +677,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="10"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="10"/>
       <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
@@ -773,27 +778,31 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="10"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="10"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
@@ -805,26 +814,57 @@
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update RTM with Test Cases
</commit_message>
<xml_diff>
--- a/RTM/RTM.xlsx
+++ b/RTM/RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>SRS_00_5</t>
   </si>
@@ -123,6 +123,19 @@
   </si>
   <si>
     <t>Application.c &amp; LCD_prog.c &amp; DIO_prog.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_3, </t>
+  </si>
+  <si>
+    <t>TC_1, TC_2
+TC_4, TC_5, TC_6</t>
+  </si>
+  <si>
+    <t>TC_7, TC_8, TC_9</t>
+  </si>
+  <si>
+    <t>TC_10</t>
   </si>
 </sst>
 </file>
@@ -205,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -229,13 +242,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -243,9 +259,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -371,6 +384,9 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -400,15 +416,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A2:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="CRS" dataDxfId="6"/>
-    <tableColumn id="2" name="SRS" dataDxfId="5"/>
-    <tableColumn id="3" name="DESIGN" dataDxfId="4"/>
-    <tableColumn id="4" name="CODE" dataDxfId="3"/>
-    <tableColumn id="5" name="TEST" dataDxfId="2"/>
-    <tableColumn id="6" name="RELATED SRS" dataDxfId="1"/>
+    <tableColumn id="1" name="CRS" dataDxfId="5"/>
+    <tableColumn id="2" name="SRS" dataDxfId="4"/>
+    <tableColumn id="3" name="DESIGN" dataDxfId="3"/>
+    <tableColumn id="4" name="CODE" dataDxfId="2"/>
+    <tableColumn id="5" name="TEST" dataDxfId="1"/>
+    <tableColumn id="6" name="RELATED SRS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -679,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,19 +705,19 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
     <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -730,11 +746,11 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
@@ -744,13 +760,15 @@
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
@@ -760,31 +778,35 @@
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
@@ -796,13 +818,15 @@
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
@@ -814,11 +838,13 @@
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="9"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update RTM with (updated test cases)
</commit_message>
<xml_diff>
--- a/RTM/RTM.xlsx
+++ b/RTM/RTM.xlsx
@@ -24,38 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
-  <si>
-    <t>SRS_00_5</t>
-  </si>
-  <si>
-    <t>SRS_00_6</t>
-  </si>
-  <si>
-    <t>SRS_00_4</t>
-  </si>
-  <si>
-    <t>CRS_00_3, CRS_00_4</t>
-  </si>
-  <si>
-    <t>SRS_00_3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
   <si>
     <t>CRS_00_1</t>
   </si>
   <si>
-    <t>SRS_00_2</t>
-  </si>
-  <si>
-    <t>SRS_00_1</t>
-  </si>
-  <si>
     <t>RELATED SRS</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
     <t>CODE</t>
   </si>
   <si>
@@ -74,78 +50,269 @@
     <t>CRS_00_6</t>
   </si>
   <si>
-    <t>CRS_00_2, CRS_00_5</t>
-  </si>
-  <si>
-    <t>SRS_00_7</t>
-  </si>
-  <si>
-    <t>CRS_00_7, CRS_00_8, CRS_00_9, CRS_00_11</t>
-  </si>
-  <si>
     <t>CRS_00_10</t>
   </si>
   <si>
-    <t>CRS_00_12, CRS_00_13, CRS_00_14</t>
-  </si>
-  <si>
-    <t>SRS_00_2, SRS_00_3</t>
-  </si>
-  <si>
-    <t>SRS_00_2, SRS_00_3, SRS_00_4</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>LCD-CDD.doc, DIO-CDD.doc</t>
-  </si>
-  <si>
     <t>App-CDD.doc</t>
   </si>
   <si>
     <t>ADC-CDD.doc, LM35-CDD</t>
   </si>
   <si>
-    <t>ADC_prog.c &amp; Volt_prog.c</t>
-  </si>
-  <si>
-    <t>LCD_prog.c &amp; DIO_prog.c</t>
-  </si>
-  <si>
     <t>Application.c</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
-    <t>App-CDD.doc &amp; LCD-CDD.doc &amp; DIO-CDD.doc</t>
-  </si>
-  <si>
-    <t>Application.c &amp; LCD_prog.c &amp; DIO_prog.c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_3, </t>
-  </si>
-  <si>
-    <t>TC_1, TC_2
-TC_4, TC_5, TC_6</t>
-  </si>
-  <si>
-    <t>TC_7, TC_8, TC_9</t>
-  </si>
-  <si>
-    <t>TC_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>SRS_1_1</t>
+  </si>
+  <si>
+    <t>SRS_2_1</t>
+  </si>
+  <si>
+    <t>SRS_3_1</t>
+  </si>
+  <si>
+    <t>SRS_4_1</t>
+  </si>
+  <si>
+    <t>SRS_5_1</t>
+  </si>
+  <si>
+    <t>SRS_6_1</t>
+  </si>
+  <si>
+    <t>SRS_7_1</t>
+  </si>
+  <si>
+    <t>SRS_8_1</t>
+  </si>
+  <si>
+    <t>SRS_9_1</t>
+  </si>
+  <si>
+    <t>SRS_10_1</t>
+  </si>
+  <si>
+    <t>SRS_11_1</t>
+  </si>
+  <si>
+    <t>SRS_12_1</t>
+  </si>
+  <si>
+    <t>SRS_13_1</t>
+  </si>
+  <si>
+    <t>TEST CASES</t>
+  </si>
+  <si>
+    <t>TC_26</t>
+  </si>
+  <si>
+    <t>TC_27</t>
+  </si>
+  <si>
+    <t>TC_31</t>
+  </si>
+  <si>
+    <t>TC_32</t>
+  </si>
+  <si>
+    <t>TC_34</t>
+  </si>
+  <si>
+    <t>SRS_NF_1</t>
+  </si>
+  <si>
+    <t>SRS_NF_2</t>
+  </si>
+  <si>
+    <t>SRS_NF_3</t>
+  </si>
+  <si>
+    <t>SRS_NF_4</t>
+  </si>
+  <si>
+    <t>SRS_NF_5</t>
+  </si>
+  <si>
+    <t>SRS_NF_6</t>
+  </si>
+  <si>
+    <t>TC_35</t>
+  </si>
+  <si>
+    <t>TC_37</t>
+  </si>
+  <si>
+    <t>TC_38</t>
+  </si>
+  <si>
+    <t>TC_39</t>
+  </si>
+  <si>
+    <t>TC_40</t>
+  </si>
+  <si>
+    <t>TC_36</t>
+  </si>
+  <si>
+    <t>TC_16</t>
+  </si>
+  <si>
+    <t>CRS_00_2</t>
+  </si>
+  <si>
+    <t>CRS_00_3</t>
+  </si>
+  <si>
+    <t>CRS_00_4</t>
+  </si>
+  <si>
+    <t>CRS_00_5</t>
+  </si>
+  <si>
+    <t>CRS_00_7</t>
+  </si>
+  <si>
+    <t>CRS_00_8</t>
+  </si>
+  <si>
+    <t>CRS_00_9</t>
+  </si>
+  <si>
+    <t>CRS_00_11</t>
+  </si>
+  <si>
+    <t>CRS_00_13</t>
+  </si>
+  <si>
+    <t>CRS_00_12, CRS_00_13</t>
+  </si>
+  <si>
+    <t>ADC_prog.c 
+ LM35_prog.c</t>
+  </si>
+  <si>
+    <t>LCD-CDD.doc
+DIO-CDD.doc</t>
+  </si>
+  <si>
+    <t>LCD_prog.c
+DIO_prog.c</t>
+  </si>
+  <si>
+    <t>Application.c
+ADC_prog.c
+LM35_prog.c
+DIO_prog.c
+LCD_prog.c</t>
+  </si>
+  <si>
+    <t>App-CDD.doc
+LCD-CDD.doc
+DIO-CDD.doc</t>
+  </si>
+  <si>
+    <t>Application.c
+LCD_prog.c
+DIO_prog.c</t>
+  </si>
+  <si>
+    <t>SRS_1_1
+SRS_2_1
+SRS_3_1
+SRS_4_1</t>
+  </si>
+  <si>
+    <t>SRS_9_1
+SRS_12_1</t>
+  </si>
+  <si>
+    <t>SRS_5_1
+SRS_9_1
+SRS_11_1</t>
+  </si>
+  <si>
+    <t>SRS_12_1
+SRS_13_1</t>
+  </si>
+  <si>
+    <t>SRS_12_1
+SRS_13_2</t>
+  </si>
+  <si>
+    <t>SRS_1_1
+SRS_2_1
+SRS_3_1
+SRS_4_1
+SRS_NF_5</t>
+  </si>
+  <si>
+    <t>SRS_1_1
+SRS_2_1
+SRS_3_1
+SRS_4_1
+SRS_NF_3</t>
+  </si>
+  <si>
+    <t>TC_1
+TC_2
+TC_3</t>
+  </si>
+  <si>
+    <t>TC_1, TC_2, TC_3
+TC_21, TC_22
+TC_23_ TC_24
+TC_25, TC_31</t>
+  </si>
+  <si>
+    <t>TC_17, TC_18
+TC_19,  TC_20</t>
+  </si>
+  <si>
+    <t>TC_33
+TC_35</t>
+  </si>
+  <si>
+    <t>TC_4, TC_5, TC_6
+TC_7, TC_8, TC_9
+TC_10, TC_11
+TC_12, TC_13
+TC_14, TC_15
+TC_16, TC_18
+TC_19</t>
+  </si>
+  <si>
+    <t>TC_28
+TC_29
+TC_30</t>
+  </si>
+  <si>
+    <t>TC_4, TC_5, TC_6
+TC_7, TC_8, TC_9
+TC_10, TC_11
+TC_12, TC_13
+TC_14, TC_15</t>
+  </si>
+  <si>
+    <t>ADC-CDD.doc
+ LM35-CDD.doc</t>
+  </si>
+  <si>
+    <t>App-CDD.doc
+LM35-CDD.doc
+ADC-CDD.doc
+LCD-CDD.doc
+DIO-CDD.doc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +335,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -183,7 +356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -206,55 +379,40 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -263,8 +421,26 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -277,11 +453,29 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -294,11 +488,29 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -311,11 +523,29 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -328,6 +558,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -341,13 +577,13 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -360,11 +596,26 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <font>
-        <sz val="14"/>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -373,7 +624,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -386,10 +637,27 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -419,14 +687,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A2:F8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:F21"/>
   <tableColumns count="6">
     <tableColumn id="1" name="CRS" dataDxfId="5"/>
     <tableColumn id="2" name="SRS" dataDxfId="4"/>
     <tableColumn id="3" name="DESIGN" dataDxfId="3"/>
     <tableColumn id="4" name="CODE" dataDxfId="2"/>
-    <tableColumn id="5" name="TEST" dataDxfId="1"/>
+    <tableColumn id="5" name="TEST CASES" dataDxfId="1"/>
     <tableColumn id="6" name="RELATED SRS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -696,206 +964,415 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="9" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="C20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19"/>
+      <c r="C21" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>